<commit_message>
[ ADD SYMBOL OF " IN ENUM SENTENCE TO AVOID SYNTAX ERROR ]
</commit_message>
<xml_diff>
--- a/dbc/CAN_VARIANT/CAN_FD_Powertrain.xlsx
+++ b/dbc/CAN_VARIANT/CAN_FD_Powertrain.xlsx
@@ -547,7 +547,7 @@
     <t>ENUM</t>
   </si>
   <si>
-    <t>no,yes</t>
+    <t>"no","yes"</t>
   </si>
   <si>
     <t>no</t>
@@ -577,7 +577,7 @@
     <t>GenMsgSendType</t>
   </si>
   <si>
-    <t>Cyclic,NotUsed,NotUsed,NotUsed,NotUsed,Cyclic,NotUsed,IfActive,NoMsgSendType,NotUsed,</t>
+    <t>"Cyclic","NotUsed","NotUsed","NotUsed","NotUsed","Cyclic","NotUsed","IfActive","NoMsgSendType","NotUsed",""</t>
   </si>
   <si>
     <t>NoMsgSendType</t>
@@ -598,7 +598,7 @@
     <t>GenMsgILSupport</t>
   </si>
   <si>
-    <t>No,Yes</t>
+    <t>"No","Yes"</t>
   </si>
   <si>
     <t>Yes</t>
@@ -613,7 +613,7 @@
     <t>CANFD_BRS</t>
   </si>
   <si>
-    <t>0,1</t>
+    <t>"0","1"</t>
   </si>
   <si>
     <t>1</t>
@@ -622,7 +622,7 @@
     <t>VFrameFormat</t>
   </si>
   <si>
-    <t>StandardCAN,ExtendedCAN,reserved,reserved,reserved,reserved,reserved,reserved,reserved,reserved,reserved,reserved,reserved,reserved,StandardCAN_FD,ExtendedCAN_FD</t>
+    <t>"StandardCAN","ExtendedCAN","reserved","reserved","reserved","reserved","reserved","reserved","reserved","reserved","reserved","reserved","reserved","reserved","StandardCAN_FD","ExtendedCAN_FD"</t>
   </si>
   <si>
     <t>StandardCAN</t>
@@ -640,7 +640,7 @@
     <t>GenSigSendType</t>
   </si>
   <si>
-    <t>Cyclic,OnWrite,OnWriteWithRepetition,OnChange,OnChangeWithRepetition,IfActive,IfActiveWithRepetition,NoSigSendType,NotUsed,NotUsed,NotUsed,NotUsed,NotUsed</t>
+    <t>"Cyclic","OnWrite","OnWriteWithRepetition","OnChange","OnChangeWithRepetition","IfActive","IfActiveWithRepetition","NoSigSendType","NotUsed","NotUsed","NotUsed","NotUsed","NotUsed"</t>
   </si>
   <si>
     <t>Cyclic</t>

</xml_diff>

<commit_message>
[ AWARE OF DEF ERROR AND THE SPACE MATTER ]
</commit_message>
<xml_diff>
--- a/dbc/CAN_VARIANT/CAN_FD_Powertrain.xlsx
+++ b/dbc/CAN_VARIANT/CAN_FD_Powertrain.xlsx
@@ -12,14 +12,14 @@
     <sheet name="ATTR" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'K-Matrix '!$A$1:$E$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'K-Matrix '!$A$1:$E$34</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2286" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2290" uniqueCount="237">
   <si>
     <t>Result</t>
   </si>
@@ -746,6 +746,9 @@
   </si>
   <si>
     <t>100 SleepInd</t>
+  </si>
+  <si>
+    <t>SIG_VALTYPE_</t>
   </si>
 </sst>
 </file>
@@ -8592,7 +8595,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E33"/>
+  <autoFilter ref="A1:E34"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -9632,7 +9635,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -10182,6 +10185,23 @@
         <v>0</v>
       </c>
     </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="C33" s="3">
+        <v>100</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>